<commit_message>
Got rid of circular import. Also, updating maze dimensions.
</commit_message>
<xml_diff>
--- a/Setup/LoadDimensions_new2021_ant.xlsx
+++ b/Setup/LoadDimensions_new2021_ant.xlsx
@@ -53,16 +53,16 @@
     <t>short edge</t>
   </si>
   <si>
-    <t>2.9</t>
-  </si>
-  <si>
-    <t>9.6</t>
-  </si>
-  <si>
     <t>4.7</t>
   </si>
   <si>
-    <t>0.8</t>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t>9.5</t>
   </si>
 </sst>
 </file>
@@ -384,7 +384,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -411,16 +411,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added method empty space for phase space.
Updated the maze dimensions.
I am still not able to calculate a solvable PhaseSpace.
</commit_message>
<xml_diff>
--- a/Setup/LoadDimensions_new2021_ant.xlsx
+++ b/Setup/LoadDimensions_new2021_ant.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -62,7 +62,10 @@
     <t>0.75</t>
   </si>
   <si>
-    <t>9.5</t>
+    <t>9.55</t>
+  </si>
+  <si>
+    <t>rounded edges</t>
   </si>
 </sst>
 </file>
@@ -381,15 +384,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -406,7 +409,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -423,19 +426,58 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>2.4</v>
+      </c>
+      <c r="C3">
+        <v>4.8</v>
+      </c>
+      <c r="D3">
+        <v>0.4</v>
+      </c>
+      <c r="E3">
+        <v>1.2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>1.2</v>
+      </c>
+      <c r="C4">
+        <v>2.9</v>
+      </c>
+      <c r="D4">
+        <v>0.2</v>
+      </c>
+      <c r="E4">
+        <v>0.6</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.6</v>
+      </c>
+      <c r="C5">
+        <v>1.2</v>
+      </c>
+      <c r="D5">
+        <v>0.1</v>
+      </c>
+      <c r="E5">
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated XL SPT ants
</commit_message>
<xml_diff>
--- a/Setup/LoadDimensions_new2021_ant.xlsx
+++ b/Setup/LoadDimensions_new2021_ant.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20136" windowHeight="8928"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20140" windowHeight="8930"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -53,19 +53,28 @@
     <t>short edge</t>
   </si>
   <si>
-    <t>4.7</t>
-  </si>
-  <si>
-    <t>2.4</t>
-  </si>
-  <si>
-    <t>0.75</t>
-  </si>
-  <si>
     <t>9.55</t>
   </si>
   <si>
     <t>rounded edges</t>
+  </si>
+  <si>
+    <t>actually measured</t>
+  </si>
+  <si>
+    <t>0.78</t>
+  </si>
+  <si>
+    <t>9.5</t>
+  </si>
+  <si>
+    <t>4.65</t>
+  </si>
+  <si>
+    <t>2.35</t>
+  </si>
+  <si>
+    <t>0.73</t>
   </si>
 </sst>
 </file>
@@ -384,15 +393,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,25 +417,40 @@
       <c r="E1" t="s">
         <v>8</v>
       </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>4.7</v>
+      </c>
+      <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="J2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
+      <c r="K2">
+        <v>2.4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -443,10 +467,10 @@
         <v>1.2</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -463,7 +487,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Updated all sizes of SPT
</commit_message>
<xml_diff>
--- a/Setup/LoadDimensions_new2021_ant.xlsx
+++ b/Setup/LoadDimensions_new2021_ant.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tabea\PycharmProjects\AntsShapes\Setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E23C91-86A7-4704-B1E5-584294A92503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20140" windowHeight="8930"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,7 +81,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -392,11 +393,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -455,19 +456,31 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2.4</v>
+        <v>2.35</v>
       </c>
       <c r="C3">
-        <v>4.8</v>
+        <v>4.75</v>
       </c>
       <c r="D3">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="E3">
-        <v>1.2</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
+      </c>
+      <c r="H3">
+        <v>2.4</v>
+      </c>
+      <c r="I3">
+        <v>4.8</v>
+      </c>
+      <c r="J3">
+        <v>0.4</v>
+      </c>
+      <c r="K3">
+        <v>1.2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -475,15 +488,27 @@
         <v>3</v>
       </c>
       <c r="B4">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C4">
+        <v>2.85</v>
+      </c>
+      <c r="D4">
+        <v>0.15</v>
+      </c>
+      <c r="E4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H4">
         <v>1.2</v>
       </c>
-      <c r="C4">
+      <c r="I4">
         <v>2.9</v>
       </c>
-      <c r="D4">
+      <c r="J4">
         <v>0.2</v>
       </c>
-      <c r="E4">
+      <c r="K4">
         <v>0.6</v>
       </c>
     </row>
@@ -492,15 +517,27 @@
         <v>4</v>
       </c>
       <c r="B5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C5">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D5">
+        <v>0.06</v>
+      </c>
+      <c r="E5">
+        <v>0.25</v>
+      </c>
+      <c r="H5">
         <v>0.6</v>
       </c>
-      <c r="C5">
+      <c r="I5">
         <v>1.2</v>
       </c>
-      <c r="D5">
+      <c r="J5">
         <v>0.1</v>
       </c>
-      <c r="E5">
+      <c r="K5">
         <v>0.3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrected the Shortest path finding algorithm.
</commit_message>
<xml_diff>
--- a/Setup/LoadDimensions_new2021_ant.xlsx
+++ b/Setup/LoadDimensions_new2021_ant.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3170" yWindow="190" windowWidth="14400" windowHeight="7360"/>
+    <workbookView xWindow="3168" yWindow="192" windowWidth="14400" windowHeight="7356"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -403,12 +403,12 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,7 +428,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -457,7 +457,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -489,7 +489,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -518,7 +518,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Improved the module to check for critical points in Configuration space. Updated the dimensions of S SPT ants.
</commit_message>
<xml_diff>
--- a/Setup/LoadDimensions_new2021_ant.xlsx
+++ b/Setup/LoadDimensions_new2021_ant.xlsx
@@ -523,16 +523,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.57999999999999996</v>
+        <v>0.6</v>
       </c>
       <c r="C5">
-        <v>1.18</v>
+        <v>1.2</v>
       </c>
       <c r="D5">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="E5">
-        <v>0.28000000000000003</v>
+        <v>0.3</v>
       </c>
       <c r="H5" s="1">
         <v>0.6</v>

</xml_diff>